<commit_message>
fix due date for outline
</commit_message>
<xml_diff>
--- a/docs/nopublish/schedule.xlsx
+++ b/docs/nopublish/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jnese\Desktop\BRT\Teaching\Intro-Data-Science\c1-intro-fall-2021\nopublish\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67054E96-3BF8-4D79-8DDC-D21160D51A6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BBC63C6-C9CE-44C1-8749-9FBDDE7827BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4068,8 +4068,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:U26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
@@ -4646,7 +4646,7 @@
         <v>44468</v>
       </c>
       <c r="D22" s="37">
-        <v>44489</v>
+        <v>44496</v>
       </c>
       <c r="E22" s="12" t="s">
         <v>203</v>

</xml_diff>

<commit_message>
add w4 video link
</commit_message>
<xml_diff>
--- a/docs/nopublish/schedule.xlsx
+++ b/docs/nopublish/schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jnese\Desktop\BRT\Teaching\Intro-Data-Science\c1-intro-fall-2021\nopublish\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F629AF5-8F22-40E9-B263-30CCD0316F22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F71E8F5-5A2D-41C8-B6EB-C4102EDB07B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="253">
   <si>
     <t>Week</t>
   </si>
@@ -787,6 +787,12 @@
   </si>
   <si>
     <t>hw4.html</t>
+  </si>
+  <si>
+    <t>https://uoregon.zoom.us/rec/share/UJo0nztb761-8FMFCcoCBxFOAy6J8LEl1oapEnbyb2zL0M0jaoXNP7cCUXDhx5gT.Q7Nszz6nLruwGZDK</t>
+  </si>
+  <si>
+    <t>qFA703i&amp;</t>
   </si>
 </sst>
 </file>
@@ -1764,31 +1770,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S23" sqref="S23"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="6.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.42578125" style="7" customWidth="1"/>
+    <col min="1" max="1" width="6.1328125" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.73046875" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.86328125" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.3984375" style="7" customWidth="1"/>
     <col min="6" max="6" width="59" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="31.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.85546875" style="7" customWidth="1"/>
+    <col min="7" max="7" width="31.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.86328125" style="7" customWidth="1"/>
     <col min="9" max="9" width="21" style="7" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="11" max="13" width="16.85546875" style="7" customWidth="1"/>
-    <col min="14" max="14" width="47.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.73046875" style="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="16.86328125" style="7" customWidth="1"/>
+    <col min="14" max="14" width="47.265625" style="7" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.265625" style="7" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="20" style="7" customWidth="1"/>
-    <col min="17" max="17" width="36.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="31.42578125" style="7" customWidth="1"/>
-    <col min="20" max="20" width="56.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="21" max="16384" width="9.140625" style="7"/>
+    <col min="17" max="17" width="36.86328125" style="7" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="31.3984375" style="7" customWidth="1"/>
+    <col min="20" max="20" width="56.73046875" style="7" bestFit="1" customWidth="1"/>
+    <col min="21" max="16384" width="9.1328125" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" s="44" customFormat="1">
@@ -1949,7 +1955,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:20" s="13" customFormat="1" ht="15.75" thickBot="1">
+    <row r="5" spans="1:20" s="13" customFormat="1" ht="14.65" thickBot="1">
       <c r="A5" s="13">
         <v>1</v>
       </c>
@@ -2385,8 +2391,12 @@
       <c r="K16" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="L16" s="1"/>
-      <c r="M16" s="1"/>
+      <c r="L16" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="M16" s="1" t="s">
+        <v>252</v>
+      </c>
       <c r="N16" s="1" t="s">
         <v>98</v>
       </c>
@@ -3180,12 +3190,12 @@
       <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="5"/>
-    <col min="2" max="2" width="16.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="100.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="52.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.1328125" style="5"/>
+    <col min="2" max="2" width="16.3984375" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="100.265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="52.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -4086,19 +4096,19 @@
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="6.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" style="9" customWidth="1"/>
-    <col min="5" max="5" width="47.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.85546875" style="7" customWidth="1"/>
-    <col min="7" max="7" width="21.85546875" style="7" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" style="7"/>
-    <col min="9" max="9" width="10.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="27.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="7"/>
+    <col min="1" max="1" width="6.1328125" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.3984375" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.265625" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.265625" style="9" customWidth="1"/>
+    <col min="5" max="5" width="47.265625" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.86328125" style="7" customWidth="1"/>
+    <col min="7" max="7" width="21.86328125" style="7" customWidth="1"/>
+    <col min="8" max="8" width="9.1328125" style="7"/>
+    <col min="9" max="9" width="10.86328125" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.1328125" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -4762,9 +4772,9 @@
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
recording 8 & render
</commit_message>
<xml_diff>
--- a/docs/nopublish/schedule.xlsx
+++ b/docs/nopublish/schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jnese\Desktop\BRT\Teaching\Intro-Data-Science\c1-intro-fall-2021\nopublish\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9DBEAF8-F18A-42BC-AF65-50E95DB06289}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{505918FB-4C56-45A0-BA34-EF0EC8F7FA0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="-60" windowWidth="19320" windowHeight="10320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="271">
   <si>
     <t>Week</t>
   </si>
@@ -841,6 +841,12 @@
   </si>
   <si>
     <t>hw9.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://uoregon.zoom.us/rec/share/RNPNqlA1ay-CfgKPSzt9fwvop0RM-PfysoF8pDxpCLuLa_tNxV5AHeUOnwO2X3cV.I-e0_W8MMDZ5Ere6 </t>
+  </si>
+  <si>
+    <t>.%+8?slH</t>
   </si>
 </sst>
 </file>
@@ -1818,31 +1824,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S38" sqref="S38"/>
+      <selection pane="bottomLeft" activeCell="M33" sqref="M33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="6.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.42578125" style="7" customWidth="1"/>
+    <col min="1" max="1" width="6.1328125" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.73046875" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.86328125" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.3984375" style="7" customWidth="1"/>
     <col min="6" max="6" width="59" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="31.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.85546875" style="7" customWidth="1"/>
+    <col min="7" max="7" width="31.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.86328125" style="7" customWidth="1"/>
     <col min="9" max="9" width="21" style="7" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="11" max="13" width="16.85546875" style="7" customWidth="1"/>
-    <col min="14" max="14" width="47.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.73046875" style="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="16.86328125" style="7" customWidth="1"/>
+    <col min="14" max="14" width="47.265625" style="7" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.265625" style="7" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="20" style="7" customWidth="1"/>
-    <col min="17" max="17" width="36.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="31.42578125" style="7" customWidth="1"/>
-    <col min="20" max="20" width="56.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="21" max="16384" width="9.140625" style="7"/>
+    <col min="17" max="17" width="36.86328125" style="7" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="31.3984375" style="7" customWidth="1"/>
+    <col min="20" max="20" width="56.73046875" style="7" bestFit="1" customWidth="1"/>
+    <col min="21" max="16384" width="9.1328125" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" s="44" customFormat="1">
@@ -2003,7 +2009,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:20" s="13" customFormat="1" ht="15.75" thickBot="1">
+    <row r="5" spans="1:20" s="13" customFormat="1" ht="14.65" thickBot="1">
       <c r="A5" s="13">
         <v>1</v>
       </c>
@@ -3015,6 +3021,12 @@
       </c>
       <c r="K33" s="1" t="s">
         <v>162</v>
+      </c>
+      <c r="L33" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="M33" s="2" t="s">
+        <v>270</v>
       </c>
       <c r="N33" s="2" t="s">
         <v>230</v>
@@ -3308,12 +3320,12 @@
       <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="5"/>
-    <col min="2" max="2" width="16.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="100.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="52.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.1328125" style="5"/>
+    <col min="2" max="2" width="16.3984375" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="100.265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="52.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -4214,19 +4226,19 @@
       <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="6.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" style="9" customWidth="1"/>
-    <col min="5" max="5" width="47.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.85546875" style="7" customWidth="1"/>
-    <col min="7" max="7" width="21.85546875" style="7" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" style="7"/>
-    <col min="9" max="9" width="10.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="27.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="7"/>
+    <col min="1" max="1" width="6.1328125" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.3984375" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.265625" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.265625" style="9" customWidth="1"/>
+    <col min="5" max="5" width="47.265625" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.86328125" style="7" customWidth="1"/>
+    <col min="7" max="7" width="21.86328125" style="7" customWidth="1"/>
+    <col min="8" max="8" width="9.1328125" style="7"/>
+    <col min="9" max="9" width="10.86328125" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.1328125" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -4911,9 +4923,9 @@
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>